<commit_message>
Tried to use Mega API, didn't work, switching to box api
</commit_message>
<xml_diff>
--- a/Classeur1_2.xlsx
+++ b/Classeur1_2.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Organizations">Feuil1!$J$3:$J$6</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>title_FR</t>
   </si>
@@ -60,6 +63,15 @@
   </si>
   <si>
     <t>ATI</t>
+  </si>
+  <si>
+    <t>LABEX</t>
+  </si>
+  <si>
+    <t>TeamEd</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -144,8 +156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G16" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G2" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
     <tableColumn id="1" uniqueName="title_FR" name="title_FR">
       <xmlColumnPr mapId="1" xpath="/section/post/title_FR" xmlDataType="string"/>
@@ -460,18 +472,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -517,10 +535,36 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>Organizations</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>